<commit_message>
chore: Update cost management mockup Excel file
</commit_message>
<xml_diff>
--- a/docs/sample data/Cost Management Mock up.xlsx
+++ b/docs/sample data/Cost Management Mock up.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\iwahbi\dev\cost-management\docs\sample data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\iwahbi\dev\cost-management-v0\docs\sample data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481B09D9-4716-4F4B-B757-1A40454AFFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919CCA77-377F-4AA3-B646-4792E40B4707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="3" xr2:uid="{03BC9608-5FA2-487C-92D0-A98DC401C2EB}"/>
+    <workbookView xWindow="2620" yWindow="2620" windowWidth="28800" windowHeight="15370" activeTab="3" xr2:uid="{03BC9608-5FA2-487C-92D0-A98DC401C2EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Spend Assumptions (3)" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="73">
   <si>
     <t>Spend Type</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>Invoice Date</t>
+  </si>
+  <si>
+    <t>Supplier Promise Date</t>
   </si>
 </sst>
 </file>
@@ -1217,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6A6112-C10C-463F-8F4C-E15087B04FE2}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:N10"/>
+      <selection sqref="A1:O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1239,9 +1242,10 @@
     <col min="12" max="12" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.453125" customWidth="1"/>
+    <col min="15" max="15" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
@@ -1284,8 +1288,11 @@
       <c r="N1" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O1" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>4584165035</v>
       </c>
@@ -1320,16 +1327,16 @@
         <v>51</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M2">
-        <v>170268.09</v>
+        <v>340536.18</v>
       </c>
       <c r="N2" s="8">
         <v>45853</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1373,7 +1380,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1417,7 +1424,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1461,7 +1468,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -1505,7 +1512,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1549,7 +1556,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1593,7 +1600,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1637,7 +1644,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -1681,7 +1688,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -1715,8 +1722,11 @@
       <c r="K11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O11" s="8">
+        <v>46037</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1750,8 +1760,11 @@
       <c r="K12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O12" s="8">
+        <v>46037</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -1785,8 +1798,11 @@
       <c r="K13" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O13" s="8">
+        <v>46037</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -1820,8 +1836,11 @@
       <c r="K14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O14" s="8">
+        <v>46037</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -1855,8 +1874,11 @@
       <c r="K15" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O15" s="8">
+        <v>46037</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -1890,8 +1912,11 @@
       <c r="K16" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="O16" s="8">
+        <v>46037</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -1925,8 +1950,11 @@
       <c r="K17" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="O17" s="8">
+        <v>46037</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -1959,6 +1987,9 @@
       </c>
       <c r="K18" t="s">
         <v>51</v>
+      </c>
+      <c r="O18" s="8">
+        <v>46037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>